<commit_message>
require_headers and skip_rows options for worksheet
</commit_message>
<xml_diff>
--- a/tests/test1.xlsx
+++ b/tests/test1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sverker\PyCharmWorkspace\telldus\excel_utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sverker\PyCharmWorkspace\openpyxl-templates\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>asdf</t>
   </si>
@@ -33,6 +33,24 @@
   </si>
   <si>
     <t>ta bort</t>
+  </si>
+  <si>
+    <t>Röd text</t>
+  </si>
+  <si>
+    <t>Svart siffra</t>
+  </si>
+  <si>
+    <t>Ytterligare en siffra</t>
+  </si>
+  <si>
+    <t>Aktion</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Tid</t>
   </si>
 </sst>
 </file>
@@ -374,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,129 +406,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>12</v>
-      </c>
-      <c r="C1">
-        <v>999</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2">
-        <v>42797</v>
-      </c>
-      <c r="F1" s="9">
-        <v>0.33333333333333331</v>
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>999</v>
       </c>
-      <c r="E2" s="3">
-        <v>42797</v>
-      </c>
-      <c r="F2" s="11">
-        <v>0.375</v>
-      </c>
-      <c r="K2" s="10"/>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>42797</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0.33333333333333331</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>999</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4">
-        <v>42797</v>
-      </c>
-      <c r="F3" s="9">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="K3" s="10">
-        <v>10001231324</v>
-      </c>
+      <c r="E3" s="3">
+        <v>42797</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4" s="7">
+        <v>10</v>
+      </c>
+      <c r="C4">
         <v>999</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="5">
-        <v>42797</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.45833333333333298</v>
+      <c r="E4" s="4">
+        <v>42797</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="K4" s="10">
+        <v>10001231324</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>999</v>
-      </c>
-      <c r="E5" s="6">
-        <v>42797</v>
-      </c>
-      <c r="F5" s="9">
-        <v>0.5</v>
+        <v>9</v>
+      </c>
+      <c r="C5" s="7">
+        <v>999</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>42797</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.45833333333333298</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>999</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>42797</v>
       </c>
       <c r="F6" s="9">
-        <v>0.54166666666666596</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>999</v>
@@ -518,19 +536,19 @@
       <c r="D7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="8">
-        <v>42797</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.58333333333333304</v>
+      <c r="E7" s="7">
+        <v>42797</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0.54166666666666596</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <v>999</v>
@@ -538,87 +556,107 @@
       <c r="D8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="8">
+      <c r="E8" s="8">
+        <v>42797</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>999</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="8">
         <v>0.625</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>4</v>
       </c>
-      <c r="C9">
-        <v>999</v>
-      </c>
-      <c r="E9" s="7">
-        <v>42797</v>
-      </c>
-      <c r="F9" s="8">
+      <c r="C10">
+        <v>999</v>
+      </c>
+      <c r="E10" s="7">
+        <v>42797</v>
+      </c>
+      <c r="F10" s="8">
         <v>0.66666666666666596</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>999</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.70833333333333304</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>999</v>
       </c>
       <c r="F11" s="2">
-        <v>0.75</v>
+        <v>0.70833333333333304</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>999</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>1</v>
       </c>
-      <c r="C12">
-        <v>999</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="C13">
+        <v>999</v>
+      </c>
+      <c r="F13" s="2">
         <v>0.79166666666666696</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F13" s="2">
-        <v>0.83333333333333304</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F14" s="2">
+        <v>0.83333333333333304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F15" s="2">
         <v>0.875</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>1</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>2</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F16" s="2">
         <v>0.91666666666666696</v>
       </c>
     </row>

</xml_diff>